<commit_message>
Finished - Have to add Comments
</commit_message>
<xml_diff>
--- a/template/template.xlsx
+++ b/template/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12392\Desktop\Github\Toast-Expense-Weekly_Sales\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2974C1CD-66A4-4A37-B34E-30318F04DAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF6B54A-F0FF-47AF-8840-DA82391B6A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5190" windowWidth="29040" windowHeight="15720" xr2:uid="{620AE1DF-7CB7-4444-94F5-28BBD257E4FD}"/>
   </bookViews>
@@ -692,7 +692,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +725,10 @@
       <c r="O1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="7"/>
+      <c r="P1" s="30">
+        <f>H5</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O2" s="6" t="s">
@@ -1594,12 +1597,18 @@
       <c r="C33" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="30"/>
+      <c r="D33" s="30">
+        <f>H5</f>
+        <v>6</v>
+      </c>
       <c r="F33" s="31"/>
       <c r="I33" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J33" s="33"/>
+      <c r="J33" s="33">
+        <f>H5</f>
+        <v>6</v>
+      </c>
       <c r="L33" s="21"/>
       <c r="M33" s="34"/>
       <c r="N33" s="24"/>

</xml_diff>